<commit_message>
pushes csvs and updated metadata excels
</commit_message>
<xml_diff>
--- a/data-raw/metadata_generated_by_flowwest/catch-metadata.xlsx
+++ b/data-raw/metadata_generated_by_flowwest/catch-metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erincain/Documents/Git/CVPIA/data-stewardship/EDI_data_repos_to_upload/rbdd-rst-edi/data-raw/metadata_generated_by_flowwest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FAAC6B7-B91D-014E-917E-7CEB18E5D14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B64CDDD-B02A-014A-81F5-E4757D081192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="1840" windowWidth="28800" windowHeight="16260" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17140" yWindow="-20800" windowWidth="19480" windowHeight="20500" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="9" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="62">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -85,9 +85,6 @@
     <t>start_time</t>
   </si>
   <si>
-    <t>site</t>
-  </si>
-  <si>
     <t>catch_id</t>
   </si>
   <si>
@@ -128,6 +125,93 @@
   </si>
   <si>
     <t xml:space="preserve">Fork length of fish caught in the trap </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start time of sample </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mortality status of fish caught in trap </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lifestage of fish caught in trap, only record lifestage for steelhead/rainbow trout </t>
+  </si>
+  <si>
+    <t xml:space="preserve">weight of fish caught in trap </t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of fish </t>
+  </si>
+  <si>
+    <t>Run of fish caught in trap, only recorded for chinook. Run determination using LAD criteria</t>
+  </si>
+  <si>
+    <t>station_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Station code indicating where trap was located, corresponds to one of the rbdd gates </t>
+  </si>
+  <si>
+    <t xml:space="preserve">count_reference </t>
+  </si>
+  <si>
+    <t>ad_pelvic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count reference column provides additional information about the LHD of fish caught in trap </t>
+  </si>
+  <si>
+    <t>enumerated</t>
+  </si>
+  <si>
+    <t>nominal</t>
+  </si>
+  <si>
+    <t>count_reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adult or Yearling fish </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juvenile YOY fish </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adipose clipped status TRUE indicates clipped adipose fin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mark used to identify  winter run out of Battle Creek TRUE indicated contains ad pelvic mark </t>
+  </si>
+  <si>
+    <t>dateTime</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ordinal </t>
+  </si>
+  <si>
+    <t>millimeter</t>
+  </si>
+  <si>
+    <t>grams</t>
+  </si>
+  <si>
+    <t>whole</t>
+  </si>
+  <si>
+    <t>real</t>
+  </si>
+  <si>
+    <t>hh:mm:ss</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD</t>
   </si>
 </sst>
 </file>
@@ -182,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -195,6 +279,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,25 +670,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AMG16385"/>
+  <dimension ref="A1:AMG16387"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="C12" sqref="C12:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="19.6640625" style="1"/>
+    <col min="1" max="1" width="19.6640625" style="1"/>
+    <col min="2" max="2" width="31.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" style="4" customWidth="1"/>
+    <col min="6" max="7" width="11.5" style="4" customWidth="1"/>
     <col min="8" max="8" width="12.1640625" style="4" customWidth="1"/>
     <col min="9" max="9" width="14.1640625" style="2" customWidth="1"/>
     <col min="10" max="10" width="16" style="4" customWidth="1"/>
     <col min="11" max="11" width="17.6640625" style="2" customWidth="1"/>
-    <col min="12" max="13" width="9.1640625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" style="4" customWidth="1"/>
     <col min="14" max="1021" width="19.6640625" style="1"/>
     <col min="1022" max="1024" width="8.33203125" customWidth="1"/>
   </cols>
@@ -641,92 +735,279 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="C2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>17</v>
+      <c r="C5" s="1" t="s">
+        <v>51</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L5" s="6">
+        <v>34533</v>
+      </c>
+      <c r="M5" s="6">
+        <v>44900</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L6" s="7">
+        <v>0</v>
+      </c>
+      <c r="M6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>18</v>
+      <c r="C7" s="1" t="s">
+        <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="E7" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="C8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0</v>
+      </c>
+      <c r="M8" s="4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>33</v>
+      <c r="B9" s="1" t="s">
+        <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="C9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0</v>
+      </c>
+      <c r="M11" s="4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
+      <c r="M12" s="4">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>19</v>
+      <c r="B15" s="1" t="s">
+        <v>49</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>28</v>
+      <c r="C15" s="1" t="s">
+        <v>45</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16"/>
+      <c r="E15" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17"/>
@@ -49835,17 +50116,23 @@
     <row r="16385" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16385"/>
     </row>
+    <row r="16386" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16386"/>
+    </row>
+    <row r="16387" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16387"/>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1020" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1022" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1020" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1022" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1020" xr:uid="{00000000-0002-0000-0800-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1022" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"ratio,interval"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -49863,7 +50150,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -49884,6 +50171,28 @@
         <v>15</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
updates nr issue and cleans up comments
</commit_message>
<xml_diff>
--- a/data-raw/metadata_generated_by_flowwest/catch-metadata.xlsx
+++ b/data-raw/metadata_generated_by_flowwest/catch-metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erincain/Documents/Git/CVPIA/data-stewardship/EDI_data_repos_to_upload/rbdd-rst-edi/data-raw/metadata_generated_by_flowwest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4328A2D3-7203-DA4C-95EB-9059A7E86C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE0D198-33DB-1749-9E4C-C16E93F1953D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17140" yWindow="-20800" windowWidth="19480" windowHeight="20500" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8180" yWindow="-20800" windowWidth="28440" windowHeight="20500" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="9" r:id="rId1"/>
@@ -18,6 +18,17 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -74,9 +85,6 @@
   </si>
   <si>
     <t>attribute_name</t>
-  </si>
-  <si>
-    <t>sample_id</t>
   </si>
   <si>
     <t>start_date</t>
@@ -175,9 +183,6 @@
     <t xml:space="preserve">Juvenile YOY fish </t>
   </si>
   <si>
-    <t xml:space="preserve">Adipose clipped status TRUE indicates clipped adipose fin </t>
-  </si>
-  <si>
     <t xml:space="preserve">Mark used to identify  winter run out of Battle Creek TRUE indicated contains ad pelvic mark </t>
   </si>
   <si>
@@ -212,6 +217,12 @@
   </si>
   <si>
     <t>gram</t>
+  </si>
+  <si>
+    <t>Adipose clipped status TRUE indicates clipped adipose fin, all ad_pelvic fish are also adipose_clipped</t>
+  </si>
+  <si>
+    <t>sample_row_id</t>
   </si>
 </sst>
 </file>
@@ -673,7 +684,7 @@
   <dimension ref="A1:AMG16387"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -737,61 +748,61 @@
     </row>
     <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="E3" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L5" s="6">
         <v>34533</v>
@@ -802,19 +813,19 @@
     </row>
     <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L6" s="7">
         <v>0</v>
@@ -825,39 +836,39 @@
     </row>
     <row r="7" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>45</v>
+      <c r="C8" s="1" t="s">
+        <v>50</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="L8" s="4">
         <v>0</v>
@@ -868,54 +879,54 @@
     </row>
     <row r="9" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>45</v>
+      <c r="C10" s="1" t="s">
+        <v>44</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>53</v>
+      <c r="E10" s="1" t="s">
+        <v>51</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>45</v>
+      <c r="C11" s="1" t="s">
+        <v>50</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="F11" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L11" s="4">
         <v>0</v>
@@ -926,25 +937,25 @@
     </row>
     <row r="12" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L12" s="4">
         <v>0</v>
@@ -955,58 +966,58 @@
     </row>
     <row r="13" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>38</v>
+      <c r="B15" s="1" t="s">
+        <v>60</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>45</v>
+      <c r="C15" s="1" t="s">
+        <v>44</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>53</v>
+      <c r="E15" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="16" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>43</v>
+      <c r="B16" s="1" t="s">
+        <v>48</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
@@ -50176,10 +50187,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -50187,10 +50198,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>